<commit_message>
Added ERGO2 application files and updated plan.
</commit_message>
<xml_diff>
--- a/management/Sem1_Plan.xlsx
+++ b/management/Sem1_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\university-git\Year 3\COMP3200 - Individual Research Project\research-project\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9DFE2F-D528-4EE5-BFC9-EEE1E572CF0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F67392-9A5A-472F-BBC7-89098A6CEA2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="12675" windowWidth="29040" windowHeight="16440" xr2:uid="{268E4CB8-1F64-4DA4-A50D-7C11BEFD8D6D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Part III Project - Semester 1</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Analyse questionnaire results</t>
   </si>
 </sst>
 </file>
@@ -311,13 +314,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Gantt Chart'!$B$6:$B$15</c15:sqref>
+                    <c15:sqref>'Gantt Chart'!$B$6:$B$16</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Gantt Chart'!$B$6:$B$9,'Gantt Chart'!$B$11:$B$15)</c:f>
+              <c:f>('Gantt Chart'!$B$6:$B$10,'Gantt Chart'!$B$12:$B$16)</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Research Lua</c:v>
                 </c:pt>
@@ -331,15 +334,18 @@
                   <c:v>Create and release Lua questionnaire</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Analyse questionnaire results</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Create a list of requirements</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Select an appropriate compiler</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Define a formal type system</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Define the program semantics</c:v>
                 </c:pt>
               </c:strCache>
@@ -350,14 +356,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Gantt Chart'!$C$6:$C$14</c15:sqref>
+                    <c15:sqref>'Gantt Chart'!$C$6:$C$15</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Gantt Chart'!$C$6:$C$9,'Gantt Chart'!$C$11:$C$14)</c:f>
+              <c:f>('Gantt Chart'!$C$6:$C$10,'Gantt Chart'!$C$12:$C$15)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>44109</c:v>
                 </c:pt>
@@ -371,15 +377,18 @@
                   <c:v>44140</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44162</c:v>
+                  <c:v>44168</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>44162</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>44173</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>44173</c:v>
                 </c:pt>
               </c:numCache>
@@ -420,13 +429,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Gantt Chart'!$B$6:$B$15</c15:sqref>
+                    <c15:sqref>'Gantt Chart'!$B$6:$B$16</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Gantt Chart'!$B$6:$B$9,'Gantt Chart'!$B$11:$B$15)</c:f>
+              <c:f>('Gantt Chart'!$B$6:$B$10,'Gantt Chart'!$B$12:$B$16)</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Research Lua</c:v>
                 </c:pt>
@@ -440,15 +449,18 @@
                   <c:v>Create and release Lua questionnaire</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Analyse questionnaire results</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Create a list of requirements</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Select an appropriate compiler</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Define a formal type system</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Define the program semantics</c:v>
                 </c:pt>
               </c:strCache>
@@ -459,36 +471,39 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Gantt Chart'!$E$6:$E$15</c15:sqref>
+                    <c15:sqref>'Gantt Chart'!$E$6:$E$16</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Gantt Chart'!$E$6:$E$9,'Gantt Chart'!$E$11:$E$15)</c:f>
+              <c:f>('Gantt Chart'!$E$6:$E$10,'Gantt Chart'!$E$12:$E$16)</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
@@ -1231,7 +1246,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1557,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5AC891-F0BD-4CC0-80D0-75BC6B4CBB6D}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1626,11 +1641,11 @@
         <v>44119</v>
       </c>
       <c r="D7" s="4">
-        <v>44155</v>
+        <v>44162</v>
       </c>
       <c r="E7" s="12">
-        <f t="shared" ref="E7:E9" si="0">D7-C7</f>
-        <v>36</v>
+        <f t="shared" ref="E7:E10" si="0">D7-C7</f>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1641,11 +1656,11 @@
         <v>44125</v>
       </c>
       <c r="D8" s="4">
-        <v>44162</v>
+        <v>44168</v>
       </c>
       <c r="E8" s="12">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1656,39 +1671,39 @@
         <v>44140</v>
       </c>
       <c r="D9" s="4">
-        <v>44162</v>
+        <v>44168</v>
       </c>
       <c r="E9" s="12">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="13"/>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4">
+        <v>44168</v>
+      </c>
+      <c r="D10" s="4">
+        <v>44173</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4">
-        <v>44162</v>
-      </c>
-      <c r="D11" s="4">
-        <v>44173</v>
-      </c>
-      <c r="E11" s="14">
-        <f>D11-C11</f>
-        <v>11</v>
-      </c>
+      <c r="B11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4">
         <v>44162</v>
@@ -1697,28 +1712,28 @@
         <v>44173</v>
       </c>
       <c r="E12" s="14">
-        <f t="shared" ref="E12:E14" si="1">D12-C12</f>
+        <f>D12-C12</f>
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4">
+        <v>44162</v>
+      </c>
+      <c r="D13" s="4">
         <v>44173</v>
       </c>
-      <c r="D13" s="4">
-        <v>44210</v>
-      </c>
       <c r="E13" s="14">
-        <f t="shared" si="1"/>
-        <v>37</v>
+        <f t="shared" ref="E13:E15" si="1">D13-C13</f>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4">
         <v>44173</v>
@@ -1731,21 +1746,36 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="15">
-        <f>MIN(C6:C14)</f>
-        <v>44109</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4">
+        <v>44173</v>
+      </c>
+      <c r="D15" s="4">
+        <v>44210</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" si="1"/>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="15">
+        <f>MIN(C6:C15)</f>
+        <v>44109</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="15">
-        <f>MAX(D6:D14)</f>
+      <c r="C29" s="15">
+        <f>MAX(D6:D15)</f>
         <v>44210</v>
       </c>
     </row>

</xml_diff>